<commit_message>
Se finaliza sección de cantidad baja
</commit_message>
<xml_diff>
--- a/Auto-Excel/Inventario.xlsx
+++ b/Auto-Excel/Inventario.xlsx
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>5</v>
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="D4" s="2" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
Agregamos 2 estadísticas al excel
</commit_message>
<xml_diff>
--- a/Auto-Excel/Inventario.xlsx
+++ b/Auto-Excel/Inventario.xlsx
@@ -1,45 +1,104 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pipe-\Documents\Miniproyectos_Python\Auto-Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8B88A6-1674-4E80-BC84-4AA36A6335F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Inventario principal" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Inventario principal" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Precio Unitario</t>
+  </si>
+  <si>
+    <t>Precio Total</t>
+  </si>
+  <si>
+    <t>Producto A</t>
+  </si>
+  <si>
+    <t>Descripción A</t>
+  </si>
+  <si>
+    <t>Producto B</t>
+  </si>
+  <si>
+    <t>Descripción B</t>
+  </si>
+  <si>
+    <t>Producto C</t>
+  </si>
+  <si>
+    <t>Descripción C</t>
+  </si>
+  <si>
+    <t>Producto D</t>
+  </si>
+  <si>
+    <t>Descripción D</t>
+  </si>
+  <si>
+    <t>Producto E</t>
+  </si>
+  <si>
+    <t>Descripción E</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFFF00"/>
-        <bgColor rgb="00FFFF00"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -56,86 +115,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -423,176 +423,140 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="4" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="10" customWidth="1" min="4" max="4"/>
-    <col width="17" customWidth="1" min="5" max="5"/>
-    <col width="14" customWidth="1" min="6" max="6"/>
+    <col min="1" max="1" width="4" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Nombre</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Descripción</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Cantidad</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Precio Unitario</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Precio Total</t>
-        </is>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>Producto A</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>Descripción A</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="n">
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2">
+        <v>100</v>
+      </c>
+      <c r="E2" s="2">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>Producto B</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Descripción B</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>Producto C</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>Descripción C</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>Producto D</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="inlineStr">
-        <is>
-          <t>Descripción D</t>
-        </is>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>Producto E</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
-        <is>
-          <t>Descripción E</t>
-        </is>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="2">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se actualizan valores de inventario
</commit_message>
<xml_diff>
--- a/Auto-Excel/Inventario.xlsx
+++ b/Auto-Excel/Inventario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pipe-\Documents\Miniproyectos_Python\Auto-Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8B88A6-1674-4E80-BC84-4AA36A6335F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA0823B-816E-4D3E-B0AB-CD3844DC7C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +471,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="2">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2">
         <v>5</v>
@@ -511,7 +511,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="2">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2">
         <v>4</v>

</xml_diff>

<commit_message>
Se importa la función en main
</commit_message>
<xml_diff>
--- a/Auto-Excel/Inventario.xlsx
+++ b/Auto-Excel/Inventario.xlsx
@@ -1,108 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pipe-\Documents\Miniproyectos_Python\Auto-Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA0823B-816E-4D3E-B0AB-CD3844DC7C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Inventario principal" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Inventario principal" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Reporte 2025-04-14" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Descripción</t>
-  </si>
-  <si>
-    <t>Cantidad</t>
-  </si>
-  <si>
-    <t>Precio Unitario</t>
-  </si>
-  <si>
-    <t>Precio Total</t>
-  </si>
-  <si>
-    <t>Producto A</t>
-  </si>
-  <si>
-    <t>Descripción A</t>
-  </si>
-  <si>
-    <t>Producto B</t>
-  </si>
-  <si>
-    <t>Descripción B</t>
-  </si>
-  <si>
-    <t>Producto C</t>
-  </si>
-  <si>
-    <t>Descripción C</t>
-  </si>
-  <si>
-    <t>Producto D</t>
-  </si>
-  <si>
-    <t>Descripción D</t>
-  </si>
-  <si>
-    <t>Producto E</t>
-  </si>
-  <si>
-    <t>Descripción E</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="000000FF"/>
+        <bgColor rgb="000000FF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -110,32 +62,110 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -423,141 +453,388 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="17" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
+    <col width="4" customWidth="1" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="17" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>Descripción</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>Cantidad</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Precio Unitario</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>Precio Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Producto A</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Descripción A</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Producto B</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Descripción B</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F3" s="2" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Producto C</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Descripción C</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F4" s="2" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Producto D</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Descripción D</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>Producto E</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>Descripción E</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2">
-        <v>10</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="F6" s="2" t="n">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Nombre</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>Descripción</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>Cantidad</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Precio Unitario</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>Precio Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Producto A</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Descripción A</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
         <v>5</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" t="n">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3">
+      <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Producto B</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Descripción B</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>20</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" t="n">
         <v>3</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" t="n">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4">
+      <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2">
-        <v>15</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Producto C</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Descripción C</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
         <v>4</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" t="n">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5">
+      <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Producto D</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Descripción D</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>30</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" t="n">
         <v>2</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" t="n">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+    <row r="6">
+      <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Producto E</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Descripción E</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
         <v>25</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" t="n">
         <v>25</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>Estadísticas</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Productos Diferentes:</t>
+        </is>
+      </c>
+      <c r="B9">
+        <f>COUNTA(B2:B6)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Total Productos:</t>
+        </is>
+      </c>
+      <c r="B10">
+        <f>SUM(D2:B6)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Valor Total del Inventario:</t>
+        </is>
+      </c>
+      <c r="B11">
+        <f>SUM(F2:F6)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se finaliza el proyecto con pruebas exitosas
</commit_message>
<xml_diff>
--- a/Auto-Excel/Inventario.xlsx
+++ b/Auto-Excel/Inventario.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Inventario principal" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Reporte 2025-04-16" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Reporte 2025-04-23" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -167,6 +167,236 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Cantidad de productos</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Inventario principal'!D1</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Inventario principal'!$A$2:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Inventario principal'!$D$2:$D$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Productos</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Cantidad de productos</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="10"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Distribución de categorías</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <pieChart>
+        <varyColors val="1"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Inventario principal'!$A$2:$A$6</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Inventario principal'!$D$2:$D$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <firstSliceAng val="0"/>
+      </pieChart>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>2</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>7</col>
+      <colOff>0</colOff>
+      <row>17</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="TablaInventario" displayName="TablaInventario" ref="A1:F6" headerRowCount="1">
+  <autoFilter ref="A1:F6"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="Nombre"/>
+    <tableColumn id="3" name="Descripción"/>
+    <tableColumn id="4" name="Cantidad"/>
+    <tableColumn id="5" name="Precio Unitario"/>
+    <tableColumn id="6" name="Precio Total"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -627,7 +857,28 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F2:F100">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="50"/>
+        <cfvo type="num" val="100"/>
+        <color rgb="00FF0000"/>
+        <color rgb="00FFFF00"/>
+        <color rgb="0000FF00"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation sqref="B2:B6" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" errorTitle="Error de validación" error="Por favor ingresar un producto correcto" type="list">
+      <formula1>"Producto A,Producto B,Producto C,Producto D,Producto E"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>